<commit_message>
Hecha de nuevo la tabla SQL de consultas al haberse actualizado los checks, y actualizado el word con conclusiones. DOCUMENTACiÖN TERMINADA :)
</commit_message>
<xml_diff>
--- a/docs/Iteracion3/CONSULTA2A.xlsx
+++ b/docs/Iteracion3/CONSULTA2A.xlsx
@@ -5,11 +5,11 @@
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jc161/Documents/GIT PROJECTS/iteracion2/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jc161/Documents/GIT PROJECTS/iteracion2/docs/Iteracion3/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="269">
   <si>
     <t>CATEGORIA</t>
   </si>
@@ -813,6 +813,27 @@
   </si>
   <si>
     <t>NOMBRETABLAREFFK</t>
+  </si>
+  <si>
+    <t>COSTO</t>
+  </si>
+  <si>
+    <t>COSTO_DE_PRODUCTO_INOF_EXISTE</t>
+  </si>
+  <si>
+    <t>FECHA_FIN</t>
+  </si>
+  <si>
+    <t>FECHA_INICIO_ANTES_DE_FIN</t>
+  </si>
+  <si>
+    <t>FECHA_INICIO</t>
+  </si>
+  <si>
+    <t>CANTIDAD_MENUS_POSITIVA</t>
+  </si>
+  <si>
+    <t>CANTIDAD_PRODUCTOS_POSITIVA</t>
   </si>
 </sst>
 </file>
@@ -1159,10 +1180,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E245"/>
+  <dimension ref="A1:E250"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B247" sqref="B247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1897,13 +1918,13 @@
         <v>68</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>72</v>
+        <v>262</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>73</v>
+        <v>263</v>
       </c>
       <c r="E47" s="1"/>
     </row>
@@ -1918,7 +1939,7 @@
         <v>17</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E48" s="1"/>
     </row>
@@ -1927,30 +1948,28 @@
         <v>68</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="E49" s="1"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>16</v>
+        <v>264</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>75</v>
+        <v>265</v>
       </c>
       <c r="E50" s="1"/>
     </row>
@@ -1959,13 +1978,13 @@
         <v>68</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>16</v>
+        <v>266</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>76</v>
+        <v>265</v>
       </c>
       <c r="E51" s="1"/>
     </row>
@@ -1974,16 +1993,16 @@
         <v>68</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -1991,10 +2010,10 @@
         <v>68</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>75</v>
@@ -2006,13 +2025,13 @@
         <v>68</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E54" s="1"/>
     </row>
@@ -2021,58 +2040,60 @@
         <v>68</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>79</v>
+        <v>13</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E55" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E56" s="1"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E57" s="1"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E58" s="1"/>
     </row>
@@ -2081,13 +2102,13 @@
         <v>63</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E59" s="1"/>
     </row>
@@ -2096,13 +2117,13 @@
         <v>63</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>1</v>
+        <v>81</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E60" s="1"/>
     </row>
@@ -2111,13 +2132,13 @@
         <v>63</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E61" s="1"/>
     </row>
@@ -2126,13 +2147,13 @@
         <v>63</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E62" s="1"/>
     </row>
@@ -2141,75 +2162,73 @@
         <v>63</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E63" s="1"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>1</v>
+        <v>88</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E64" s="1"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>1</v>
+        <v>88</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E65" s="1"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>13</v>
+        <v>88</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>29</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="E66" s="1"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E67" s="1"/>
     </row>
@@ -2218,13 +2237,13 @@
         <v>11</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E68" s="1"/>
     </row>
@@ -2233,58 +2252,60 @@
         <v>11</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>79</v>
+        <v>13</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E69" s="1"/>
+        <v>91</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>94</v>
+        <v>13</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E70" s="1"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>94</v>
+        <v>13</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E71" s="1"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E72" s="1"/>
     </row>
@@ -2293,13 +2314,13 @@
         <v>47</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E73" s="1"/>
     </row>
@@ -2308,7 +2329,7 @@
         <v>47</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>17</v>
@@ -2323,13 +2344,13 @@
         <v>47</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E75" s="1"/>
     </row>
@@ -2338,13 +2359,13 @@
         <v>47</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E76" s="1"/>
     </row>
@@ -2353,92 +2374,90 @@
         <v>47</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="E77" s="1"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E78" s="1"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>104</v>
+        <v>47</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E79" s="1"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>104</v>
+        <v>47</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>107</v>
+        <v>39</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E80" s="1"/>
+        <v>102</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>104</v>
+        <v>47</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="E81" s="1"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>9</v>
+        <v>105</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>110</v>
+        <v>267</v>
       </c>
       <c r="E82" s="1"/>
     </row>
@@ -2447,13 +2466,13 @@
         <v>104</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>9</v>
+        <v>105</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E83" s="1"/>
     </row>
@@ -2462,45 +2481,45 @@
         <v>104</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>13</v>
+        <v>107</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="E84" s="1"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E85" s="1"/>
+        <v>109</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E86" s="1"/>
     </row>
@@ -2509,39 +2528,39 @@
         <v>104</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>113</v>
+        <v>9</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>40</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="E87" s="1"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>113</v>
+        <v>13</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E88" s="1"/>
+        <v>109</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>113</v>
+        <v>13</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>2</v>
@@ -2553,63 +2572,63 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>105</v>
+        <v>13</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E90" s="1"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E91" s="1"/>
+        <v>114</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>16</v>
+        <v>113</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>68</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="E92" s="1"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>16</v>
+        <v>113</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="E93" s="1"/>
     </row>
@@ -2618,13 +2637,13 @@
         <v>116</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>16</v>
+        <v>105</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E94" s="1"/>
     </row>
@@ -2633,30 +2652,28 @@
         <v>116</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>13</v>
+        <v>105</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>68</v>
-      </c>
+        <v>268</v>
+      </c>
+      <c r="E95" s="1"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>116</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>13</v>
+        <v>107</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E96" s="1"/>
     </row>
@@ -2665,45 +2682,45 @@
         <v>116</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E97" s="1"/>
+        <v>119</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>116</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>113</v>
+        <v>16</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>40</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="E98" s="1"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>116</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>113</v>
+        <v>16</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E99" s="1"/>
     </row>
@@ -2712,92 +2729,92 @@
         <v>116</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>113</v>
+        <v>13</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E100" s="1"/>
+        <v>119</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>126</v>
+        <v>13</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>68</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="E101" s="1"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>126</v>
+        <v>13</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="E102" s="1"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E103" s="1"/>
+        <v>123</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>9</v>
+        <v>113</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="E104" s="1"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>9</v>
+        <v>113</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="E105" s="1"/>
     </row>
@@ -2806,156 +2823,156 @@
         <v>125</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>9</v>
+        <v>126</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E106" s="1"/>
+        <v>127</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>125</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>13</v>
+        <v>126</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="E107" s="1"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>125</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>13</v>
+        <v>126</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>68</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="E108" s="1"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>125</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E109" s="1"/>
+        <v>130</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>125</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E110" s="1"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E111" s="1" t="s">
-        <v>63</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="E111" s="1"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E112" s="1"/>
+        <v>130</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E113" s="1"/>
+        <v>127</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>126</v>
+        <v>13</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E114" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="E114" s="1"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>126</v>
+        <v>13</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E115" s="1"/>
     </row>
@@ -2964,90 +2981,92 @@
         <v>133</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>126</v>
+        <v>61</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E116" s="1"/>
+        <v>134</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E117" s="1" t="s">
-        <v>46</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="E117" s="1"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E118" s="1"/>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E119" s="1"/>
+        <v>137</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="E120" s="1"/>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E121" s="1"/>
     </row>
@@ -3056,19 +3075,21 @@
         <v>139</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>145</v>
+        <v>44</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E122" s="1"/>
+        <v>140</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>44</v>
@@ -3077,79 +3098,73 @@
         <v>17</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E123" s="1" t="s">
-        <v>139</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="E123" s="1"/>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>44</v>
+        <v>142</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="E124" s="1"/>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E125" s="1" t="s">
-        <v>0</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="E125" s="1"/>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E126" s="1"/>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>44</v>
+        <v>145</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E127" s="1" t="s">
-        <v>139</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="E127" s="1"/>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>44</v>
@@ -3158,114 +3173,120 @@
         <v>17</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="E128" s="1"/>
+        <v>148</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>155</v>
+        <v>44</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E129" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="E129" s="1"/>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="E130" s="1"/>
+        <v>151</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>19</v>
+        <v>147</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>81</v>
+        <v>150</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="E131" s="1"/>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>19</v>
+        <v>152</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E132" s="1"/>
+        <v>153</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>19</v>
+        <v>152</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="E133" s="1"/>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>19</v>
+        <v>152</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>85</v>
+        <v>155</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="E134" s="1"/>
+        <v>156</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>19</v>
+        <v>152</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>1</v>
+        <v>155</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="E135" s="1"/>
     </row>
@@ -3274,13 +3295,13 @@
         <v>19</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>162</v>
+        <v>81</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="E136" s="1"/>
     </row>
@@ -3289,13 +3310,13 @@
         <v>19</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>162</v>
+        <v>81</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="E137" s="1"/>
     </row>
@@ -3304,30 +3325,28 @@
         <v>19</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>165</v>
+        <v>81</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="E138" s="1" t="s">
-        <v>167</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="E138" s="1"/>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>165</v>
+        <v>85</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="E139" s="1"/>
     </row>
@@ -3336,13 +3355,13 @@
         <v>19</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="E140" s="1"/>
     </row>
@@ -3351,13 +3370,13 @@
         <v>19</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>88</v>
+        <v>162</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="E141" s="1"/>
     </row>
@@ -3366,241 +3385,241 @@
         <v>19</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>88</v>
+        <v>162</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="E142" s="1"/>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>169</v>
+        <v>19</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>41</v>
+        <v>165</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="E143" s="1"/>
+        <v>166</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>169</v>
+        <v>19</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="E144" s="1" t="s">
-        <v>46</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="E144" s="1"/>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>169</v>
+        <v>19</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>171</v>
+        <v>88</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="E145" s="1"/>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>169</v>
+        <v>19</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E146" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="E146" s="1"/>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>169</v>
+        <v>19</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>13</v>
+        <v>88</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E147" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="E147" s="1"/>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>169</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>174</v>
+        <v>41</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="E148" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="E148" s="1"/>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>169</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="E149" s="1"/>
+        <v>172</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>29</v>
+        <v>169</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="E150" s="1" t="s">
-        <v>46</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="E150" s="1"/>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>29</v>
+        <v>169</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>178</v>
+        <v>9</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="E151" s="1"/>
+        <v>173</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>29</v>
+        <v>169</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E152" s="1"/>
+        <v>173</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>29</v>
+        <v>169</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>1</v>
+        <v>174</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E153" s="1"/>
+        <v>175</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>29</v>
+        <v>169</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E154" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="E154" s="1"/>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E155" s="1"/>
+        <v>179</v>
+      </c>
+      <c r="E155" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>185</v>
+        <v>29</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>1</v>
+        <v>178</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="E156" s="1"/>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>185</v>
+        <v>29</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>1</v>
@@ -3609,86 +3628,84 @@
         <v>2</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="E157" s="1"/>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>188</v>
+        <v>29</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>189</v>
+        <v>1</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E158" s="1" t="s">
-        <v>63</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="E158" s="1"/>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>188</v>
+        <v>29</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E159" s="1"/>
+        <v>183</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>188</v>
+        <v>29</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="E160" s="1"/>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E161" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="E161" s="1"/>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E162" s="1"/>
     </row>
@@ -3697,45 +3714,45 @@
         <v>188</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>16</v>
+        <v>189</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="E163" s="1"/>
+        <v>190</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>188</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E164" s="1" t="s">
-        <v>63</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="E164" s="1"/>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>188</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E165" s="1"/>
     </row>
@@ -3744,45 +3761,45 @@
         <v>188</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>195</v>
+        <v>16</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="E166" s="1"/>
+        <v>193</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>188</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="E167" s="1" t="s">
-        <v>104</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="E167" s="1"/>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>188</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="E168" s="1"/>
     </row>
@@ -3791,45 +3808,45 @@
         <v>188</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>9</v>
+        <v>195</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E169" s="1"/>
+        <v>196</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>188</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>13</v>
+        <v>195</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="E170" s="1" t="s">
-        <v>104</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="E170" s="1"/>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>188</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>13</v>
+        <v>195</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="E171" s="1"/>
     </row>
@@ -3838,45 +3855,45 @@
         <v>188</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C172" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E172" s="1"/>
+        <v>198</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>188</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>113</v>
+        <v>9</v>
       </c>
       <c r="C173" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="E173" s="1" t="s">
-        <v>104</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="E173" s="1"/>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>188</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>113</v>
+        <v>9</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="E174" s="1"/>
     </row>
@@ -3885,92 +3902,92 @@
         <v>188</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>113</v>
+        <v>13</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="E175" s="1"/>
+        <v>198</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>189</v>
+        <v>13</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="E176" s="1" t="s">
-        <v>63</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="E176" s="1"/>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>189</v>
+        <v>13</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E177" s="1"/>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>189</v>
+        <v>113</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="E178" s="1"/>
+        <v>198</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>16</v>
+        <v>113</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="E179" s="1" t="s">
-        <v>116</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="E179" s="1"/>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>16</v>
+        <v>113</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E180" s="1"/>
     </row>
@@ -3979,45 +3996,45 @@
         <v>202</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>16</v>
+        <v>189</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="E181" s="1"/>
+        <v>203</v>
+      </c>
+      <c r="E181" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>202</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="E182" s="1" t="s">
-        <v>63</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="E182" s="1"/>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>202</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C183" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E183" s="1"/>
     </row>
@@ -4026,45 +4043,45 @@
         <v>202</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>195</v>
+        <v>16</v>
       </c>
       <c r="C184" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="E184" s="1"/>
+        <v>206</v>
+      </c>
+      <c r="E184" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>202</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="E185" s="1" t="s">
-        <v>116</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="E185" s="1"/>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>202</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="E186" s="1"/>
     </row>
@@ -4073,45 +4090,45 @@
         <v>202</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>13</v>
+        <v>195</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="E187" s="1"/>
+        <v>208</v>
+      </c>
+      <c r="E187" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>202</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>113</v>
+        <v>195</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="E188" s="1" t="s">
-        <v>116</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="E188" s="1"/>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
         <v>202</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>113</v>
+        <v>195</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="E189" s="1"/>
     </row>
@@ -4120,92 +4137,92 @@
         <v>202</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>113</v>
+        <v>13</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="E190" s="1"/>
+        <v>206</v>
+      </c>
+      <c r="E190" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>189</v>
+        <v>13</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="E191" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="E191" s="1"/>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>189</v>
+        <v>13</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E192" s="1"/>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>189</v>
+        <v>113</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="E193" s="1"/>
+        <v>206</v>
+      </c>
+      <c r="E193" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>195</v>
+        <v>113</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="E194" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="E194" s="1"/>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>195</v>
+        <v>113</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E195" s="1"/>
     </row>
@@ -4214,45 +4231,45 @@
         <v>212</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="E196" s="1"/>
+        <v>213</v>
+      </c>
+      <c r="E196" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
         <v>212</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>9</v>
+        <v>189</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E197" s="1" t="s">
-        <v>104</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="E197" s="1"/>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
         <v>212</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>9</v>
+        <v>189</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E198" s="1"/>
     </row>
@@ -4261,45 +4278,45 @@
         <v>212</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>9</v>
+        <v>195</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="E199" s="1"/>
+        <v>216</v>
+      </c>
+      <c r="E199" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
         <v>212</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>13</v>
+        <v>195</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E200" s="1" t="s">
-        <v>104</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="E200" s="1"/>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
         <v>212</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>13</v>
+        <v>195</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="E201" s="1"/>
     </row>
@@ -4308,45 +4325,45 @@
         <v>212</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="E202" s="1"/>
+        <v>218</v>
+      </c>
+      <c r="E202" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
         <v>212</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>113</v>
+        <v>9</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E203" s="1" t="s">
-        <v>104</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="E203" s="1"/>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
         <v>212</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>113</v>
+        <v>9</v>
       </c>
       <c r="C204" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="E204" s="1"/>
     </row>
@@ -4355,122 +4372,124 @@
         <v>212</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>113</v>
+        <v>13</v>
       </c>
       <c r="C205" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E205" s="1"/>
+        <v>218</v>
+      </c>
+      <c r="E205" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="E206" s="1" t="s">
-        <v>60</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="E206" s="1"/>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E207" s="1"/>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>61</v>
+        <v>113</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="E208" s="1"/>
+        <v>218</v>
+      </c>
+      <c r="E208" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>61</v>
+        <v>113</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="E209" s="1"/>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>195</v>
+        <v>113</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="E210" s="1" t="s">
-        <v>63</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="E210" s="1"/>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
         <v>222</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>195</v>
+        <v>61</v>
       </c>
       <c r="C211" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="E211" s="1"/>
+        <v>223</v>
+      </c>
+      <c r="E211" s="1" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
         <v>222</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>195</v>
+        <v>61</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E212" s="1"/>
     </row>
@@ -4479,13 +4498,13 @@
         <v>222</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>195</v>
+        <v>61</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E213" s="1"/>
     </row>
@@ -4494,154 +4513,154 @@
         <v>222</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="E214" s="1" t="s">
-        <v>60</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="E214" s="1"/>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
         <v>222</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>13</v>
+        <v>195</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="E215" s="1"/>
+        <v>227</v>
+      </c>
+      <c r="E215" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
         <v>222</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>13</v>
+        <v>195</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="E216" s="1"/>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>16</v>
+        <v>195</v>
       </c>
       <c r="C217" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="E217" s="1" t="s">
-        <v>68</v>
-      </c>
+        <v>225</v>
+      </c>
+      <c r="E217" s="1"/>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>16</v>
+        <v>195</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E218" s="1"/>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="E219" s="1"/>
+        <v>223</v>
+      </c>
+      <c r="E219" s="1" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="E220" s="1"/>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>195</v>
+        <v>13</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="E221" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>229</v>
+      </c>
+      <c r="E221" s="1"/>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
         <v>230</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>195</v>
+        <v>16</v>
       </c>
       <c r="C222" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="E222" s="1"/>
+        <v>231</v>
+      </c>
+      <c r="E222" s="1" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
         <v>230</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>195</v>
+        <v>16</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E223" s="1"/>
     </row>
@@ -4650,13 +4669,13 @@
         <v>230</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>195</v>
+        <v>16</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E224" s="1"/>
     </row>
@@ -4665,227 +4684,229 @@
         <v>230</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="E225" s="1" t="s">
-        <v>68</v>
-      </c>
+        <v>234</v>
+      </c>
+      <c r="E225" s="1"/>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
         <v>230</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>13</v>
+        <v>195</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="E226" s="1"/>
+        <v>235</v>
+      </c>
+      <c r="E226" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
         <v>230</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>13</v>
+        <v>195</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="E227" s="1"/>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
-        <v>167</v>
+        <v>230</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>1</v>
+        <v>195</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="E228" s="1"/>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
-        <v>167</v>
+        <v>230</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>1</v>
+        <v>195</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E229" s="1"/>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
-        <v>46</v>
+        <v>230</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="E230" s="1"/>
+        <v>231</v>
+      </c>
+      <c r="E230" s="1" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
-        <v>46</v>
+        <v>230</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="E231" s="1"/>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
-        <v>46</v>
+        <v>230</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="E232" s="1"/>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
-        <v>46</v>
+        <v>167</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>185</v>
+        <v>1</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="E233" s="1" t="s">
-        <v>185</v>
-      </c>
+        <v>238</v>
+      </c>
+      <c r="E233" s="1"/>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
-        <v>46</v>
+        <v>167</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>185</v>
+        <v>1</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="E234" s="1"/>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>245</v>
+        <v>85</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="E235" s="1"/>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>245</v>
+        <v>85</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="E236" s="1"/>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>94</v>
+        <v>1</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="E237" s="1"/>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>94</v>
+        <v>185</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="E238" s="1"/>
+        <v>243</v>
+      </c>
+      <c r="E238" s="1" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>94</v>
+        <v>185</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="E239" s="1"/>
     </row>
@@ -4894,13 +4915,13 @@
         <v>39</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>98</v>
+        <v>245</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="E240" s="1"/>
     </row>
@@ -4909,13 +4930,13 @@
         <v>39</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>98</v>
+        <v>245</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E241" s="1"/>
     </row>
@@ -4924,13 +4945,13 @@
         <v>39</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C242" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E242" s="1"/>
     </row>
@@ -4939,13 +4960,13 @@
         <v>39</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>253</v>
+        <v>94</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="E243" s="1"/>
     </row>
@@ -4954,13 +4975,13 @@
         <v>39</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>253</v>
+        <v>94</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="E244" s="1"/>
     </row>
@@ -4969,15 +4990,90 @@
         <v>39</v>
       </c>
       <c r="B245" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C245" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D245" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E245" s="1"/>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A246" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D246" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E246" s="1"/>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A247" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C247" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D247" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="E247" s="1"/>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A248" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B248" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C248" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D248" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E248" s="1"/>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A249" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B249" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C249" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D249" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E249" s="1"/>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A250" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B250" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C245" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D245" s="1" t="s">
+      <c r="C250" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D250" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="E245" s="1"/>
+      <c r="E250" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Re estructuración excel consulta 2A.
</commit_message>
<xml_diff>
--- a/docs/Iteracion3/CONSULTA2A.xlsx
+++ b/docs/Iteracion3/CONSULTA2A.xlsx
@@ -1183,14 +1183,14 @@
   <dimension ref="A1:E250"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B247" sqref="B247"/>
+      <selection activeCell="D133" sqref="D133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.83203125" customWidth="1"/>
-    <col min="2" max="2" width="24.83203125" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" customWidth="1"/>
+    <col min="1" max="1" width="30.1640625" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" customWidth="1"/>
     <col min="4" max="4" width="27.6640625" customWidth="1"/>
     <col min="5" max="5" width="18.5" customWidth="1"/>
   </cols>

</xml_diff>